<commit_message>
migrate request with adjusted end date
</commit_message>
<xml_diff>
--- a/test/test_data/test_data_IZ_to_IZ_1.xlsx
+++ b/test/test_data/test_data_IZ_to_IZ_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RaphaëlRey\PycharmProjects\iz_to_iz_transfer\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A026DEDE-D2F6-4AEF-BEAD-B4156E7A2079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D050491-4696-49E1-B5B5-244E149B994F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="800" activeTab="6" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
+    <workbookView xWindow="-17595" yWindow="3780" windowWidth="14400" windowHeight="8175" tabRatio="800" xr2:uid="{AD365A3D-3304-46D8-98A5-452209B6D1C5}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -970,8 +970,8 @@
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
@@ -1120,7 +1120,7 @@
         <v>159</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2046,7 +2046,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>